<commit_message>
Update files according to new changes.
</commit_message>
<xml_diff>
--- a/Country.xlsx
+++ b/Country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://denveru-my.sharepoint.com/personal/kexin_shang_du_edu/Documents/Pardee 2024 Winter/FAO_FBS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panda\OneDrive - University of Denver\Pardee 2024 Winter\FAO_FBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_645581EA66EB0C07292C4C5E9D6E342178784EDB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21DB4832-0172-4FC6-AD0E-0B2941FD6C64}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECBB85C-34D0-4194-8041-8D97D288EBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="3060" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -2042,7 +2042,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2054,6 +2054,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2094,11 +2101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2646,8 +2654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5366EC4-01FF-4612-85E0-FD3D66D9101C}">
   <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3027,24 +3035,24 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4724,43 +4732,46 @@
     <cfRule type="duplicateValues" dxfId="22" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C122">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95">
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
     <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  <conditionalFormatting sqref="C113">
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C122">
+    <cfRule type="duplicateValues" dxfId="8" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159:C160">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
@@ -4771,20 +4782,17 @@
   <conditionalFormatting sqref="C167">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C169">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C176">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C181">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C169">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C186">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C113">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7245,7 +7253,7 @@
   </sheetData>
   <autoFilter ref="A1:C222" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>